<commit_message>
se arreglaron las consultas de las tablas con la base de datos
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/frecebera.xlsx
+++ b/QYMSAS/bin/Debug/temp/frecebera.xlsx
@@ -42,13 +42,13 @@
     <x:t>FECHA INICIAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>1/02/2019</x:t>
+    <x:t>28/02/2019</x:t>
   </x:si>
   <x:si>
     <x:t>FECHA FINAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>26/05/2021</x:t>
+    <x:t>30/05/2021</x:t>
   </x:si>
   <x:si>
     <x:t>CANTERA EL CUCHARO</x:t>
@@ -1121,7 +1121,7 @@
       <x:c r="I14" s="6" t="s"/>
       <x:c r="J14" s="6" t="s"/>
       <x:c r="K14" s="5" t="n">
-        <x:v>143</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L14" s="5" t="s"/>
       <x:c r="M14" s="4" t="s"/>
@@ -1140,7 +1140,7 @@
       <x:c r="I15" s="6" t="s"/>
       <x:c r="J15" s="6" t="s"/>
       <x:c r="K15" s="5" t="n">
-        <x:v>12760000</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L15" s="5" t="s"/>
       <x:c r="M15" s="4" t="s"/>
@@ -1167,7 +1167,7 @@
       <x:c r="I17" s="6" t="s"/>
       <x:c r="J17" s="6" t="s"/>
       <x:c r="K17" s="5" t="n">
-        <x:v>2325000</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L17" s="5" t="s"/>
       <x:c r="M17" s="4" t="s"/>
@@ -1194,7 +1194,7 @@
       <x:c r="I19" s="6" t="s"/>
       <x:c r="J19" s="6" t="s"/>
       <x:c r="K19" s="5" t="n">
-        <x:v>1200000</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="L19" s="5" t="s"/>
       <x:c r="M19" s="4" t="s"/>

</xml_diff>